<commit_message>
TB Code and Sample error file
</commit_message>
<xml_diff>
--- a/ClientFiles/EMS FLASH SALE DATA ENTRY MODULE_DataValidation 1 (4).xlsx
+++ b/ClientFiles/EMS FLASH SALE DATA ENTRY MODULE_DataValidation 1 (4).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bellona\BellonaUtilities\Bellona\ClientFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E42971-A800-40C2-9880-AC8DEFB499D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E445FABC-90A9-41F6-A678-53B0F196FD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,6 +39,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -950,6 +972,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -968,12 +1005,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -981,15 +1012,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1393,9 +1415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:C1"/>
+      <selection pane="topRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1416,68 +1438,68 @@
       <c r="A1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="22">
         <v>45554</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="25">
+      <c r="C1" s="23"/>
+      <c r="D1" s="22">
         <v>45555</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="25">
+      <c r="E1" s="23"/>
+      <c r="F1" s="22">
         <v>45557</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="19">
+      <c r="G1" s="23"/>
+      <c r="H1" s="24">
         <v>45554</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="19">
+      <c r="I1" s="25"/>
+      <c r="J1" s="24">
         <v>45555</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="19">
+      <c r="K1" s="25"/>
+      <c r="L1" s="24">
         <v>45557</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="21">
+      <c r="M1" s="25"/>
+      <c r="N1" s="26">
         <v>45554</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21">
+      <c r="O1" s="26"/>
+      <c r="P1" s="26">
         <v>45555</v>
       </c>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21">
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26">
         <v>45557</v>
       </c>
-      <c r="S1" s="21"/>
+      <c r="S1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="22" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="24"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
@@ -2244,11 +2266,17 @@
       <c r="B25" s="12">
         <v>1202.8</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="12">
+        <f>SUM(B18:B22)/B24</f>
+        <v>1202.8021276595744</v>
+      </c>
       <c r="D25" s="12">
         <v>1589.38</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="12" t="e" cm="1">
+        <f t="array" aca="1" ref="E25" ca="1">D22()</f>
+        <v>#REF!</v>
+      </c>
       <c r="F25" s="12">
         <v>1170.51</v>
       </c>
@@ -3571,18 +3599,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="H2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C54">
     <cfRule type="containsBlanks" priority="23" stopIfTrue="1">

</xml_diff>